<commit_message>
update the feature list
</commit_message>
<xml_diff>
--- a/product/emqx_products_features_list.xlsx
+++ b/product/emqx_products_features_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rockyjin/Downloads/EMQ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rockyjin/Downloads/workspace/emqx/internal-docs/product/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="228">
   <si>
     <t>Session management and offline messages</t>
   </si>
@@ -1006,6 +1006,46 @@
   </si>
   <si>
     <t>EMQ X Production Features Comparison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>InfluxDB消息存储</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据桥接到Apache Pulsar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenTSDB消息存储</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Data persistence to InfluxDB </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data persistence TimeScaleDB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data bridge to Apache Pulsar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data persistence to AWS Dynamodb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeScaleDB消息存储</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWS Dynamodb消息存储</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1214,10 +1254,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1226,8 +1266,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -1338,7 +1378,7 @@
         <xdr:cNvPr id="2" name="officeArt object">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1392,7 +1432,7 @@
         <xdr:cNvPr id="2" name="officeArt object">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1723,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="118" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="118" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,12 +1778,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
@@ -2453,7 +2493,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6" t="s">
@@ -2465,7 +2505,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>80</v>
+        <v>218</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6" t="s">
@@ -2476,10 +2516,9 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="6"/>
+      <c r="A59" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="C59" s="6" t="s">
         <v>17</v>
       </c>
@@ -2488,10 +2527,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" s="6"/>
+      <c r="A60" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="C60" s="6" t="s">
         <v>17</v>
       </c>
@@ -2501,7 +2539,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
@@ -2513,7 +2551,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
@@ -2524,46 +2562,44 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="8" t="s">
+      <c r="C65" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B66" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="8" t="s">
@@ -2575,19 +2611,21 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
@@ -2599,7 +2637,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
@@ -2611,99 +2649,101 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
       <c r="B70" s="6"/>
-      <c r="C70" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="8" t="s">
+      <c r="C70" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="A71" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B76" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="C76" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
+        <v>195</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="D77" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
@@ -2712,38 +2752,34 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="6" t="s">
+      <c r="A79" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B80" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="C80" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>57</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
         <v>57</v>
       </c>
@@ -2753,27 +2789,31 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B82" s="6"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5" t="s">
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
@@ -2781,31 +2821,41 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="29" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="29" t="s">
         <v>212</v>
-      </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="30" t="s">
-        <v>213</v>
       </c>
       <c r="B87" s="29"/>
       <c r="C87" s="29"/>
       <c r="D87" s="29"/>
     </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A86:D86"/>
     <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A88:D88"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A87" r:id="rId1"/>
+    <hyperlink ref="A88" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -2814,27 +2864,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A45" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.83203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="16" style="22" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="22" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
@@ -3577,7 +3627,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B58" s="20"/>
       <c r="C58" s="20" t="s">
@@ -3588,32 +3638,32 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="20" t="s">
+      <c r="A59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>142</v>
+        <v>225</v>
       </c>
       <c r="B60" s="20"/>
       <c r="C60" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B61" s="20"/>
       <c r="C61" s="20" t="s">
@@ -3625,53 +3675,55 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
+      <c r="C62" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="21" t="s">
+      <c r="C65" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C66" s="21" t="s">
@@ -3683,19 +3735,21 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B68" s="20"/>
       <c r="C68" s="20" t="s">
@@ -3707,7 +3761,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B69" s="20"/>
       <c r="C69" s="20" t="s">
@@ -3719,137 +3773,135 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B70" s="20"/>
-      <c r="C70" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="21" t="s">
+      <c r="C70" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="18" t="s">
+      <c r="A71" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B73" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="20" t="s">
         <v>57</v>
       </c>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B76" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C75" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="18" t="s">
+      <c r="C76" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B77" s="18"/>
-      <c r="C77" s="18"/>
+        <v>157</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="D77" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>202</v>
+        <v>158</v>
       </c>
       <c r="B78" s="18"/>
       <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
+      <c r="D78" s="18" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B79" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="A79" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" s="20"/>
+        <v>64</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C80" s="20" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>67</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B81" s="20"/>
       <c r="C81" s="20" t="s">
         <v>67</v>
       </c>
@@ -3859,27 +3911,31 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
-      <c r="D83" s="18" t="s">
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B84" s="18"/>
       <c r="C84" s="18"/>
@@ -3887,39 +3943,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="29" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="29" t="s">
         <v>215</v>
-      </c>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="30" t="s">
-        <v>214</v>
       </c>
       <c r="B87" s="29"/>
       <c r="C87" s="29"/>
       <c r="D87" s="29"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
+      <c r="A88" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89" s="14"/>
       <c r="D89" s="14"/>
     </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A86:D86"/>
     <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A88:D88"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A87" r:id="rId1"/>
+    <hyperlink ref="A88" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -4767,7 +4833,7 @@
       </c>
       <c r="B91" s="32"/>
       <c r="C91" s="32"/>
-      <c r="D91" s="31"/>
+      <c r="D91" s="27"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="30" t="s">
@@ -4775,7 +4841,7 @@
       </c>
       <c r="B92" s="30"/>
       <c r="C92" s="30"/>
-      <c r="D92" s="31"/>
+      <c r="D92" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5645,7 +5711,7 @@
       </c>
       <c r="B92" s="29"/>
       <c r="C92" s="29"/>
-      <c r="D92" s="31"/>
+      <c r="D92" s="27"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="30" t="s">
@@ -5653,7 +5719,7 @@
       </c>
       <c r="B93" s="30"/>
       <c r="C93" s="30"/>
-      <c r="D93" s="31"/>
+      <c r="D93" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>